<commit_message>
Bento local search scripts v1
</commit_message>
<xml_diff>
--- a/InputFiles/TC06_Canine_Filter_Study-MGT01.xlsx
+++ b/InputFiles/TC06_Canine_Filter_Study-MGT01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9761D1FA-F6EE-4EF4-B249-3F22B5C1F633}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1675E015-29CE-4797-94FF-7B04C01B1C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView minimized="1" xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -467,19 +467,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.77734375" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.28515625" customWidth="1"/>
+    <col min="5" max="5" width="50" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -496,7 +496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -513,7 +513,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -530,7 +530,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="255" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>

</xml_diff>